<commit_message>
Findings for Volume of sale and Prob. of sale analyses Added SQL query measuring the signalled parameters
</commit_message>
<xml_diff>
--- a/analyses/Analyse_Ergebnisse.xlsx
+++ b/analyses/Analyse_Ergebnisse.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Masterarbeit-WebScraper\WebScraper\analyses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737678CE-164F-426B-BDD5-87410A102A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C9013A-0B24-43E5-80D7-9F2BF10732EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Verkaufsvolumen nach Auktion" sheetId="2" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
+    <sheet name="Signalattribute" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="ExterneDaten_1" localSheetId="0" hidden="1">'Verkaufsvolumen nach Auktion'!$A$1:$C$40</definedName>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>auctiondate</t>
   </si>
@@ -67,6 +67,141 @@
   <si>
     <t>prob_of_sale</t>
   </si>
+  <si>
+    <t>Findings:</t>
+  </si>
+  <si>
+    <t>Median vor Corona:</t>
+  </si>
+  <si>
+    <t>Median während Corona</t>
+  </si>
+  <si>
+    <t>Letzte Präsenzauktion</t>
+  </si>
+  <si>
+    <t>URL: 431</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Handelsvolumen (Price_sum blau) der Plattform steigt drastisch am 17.02.2021 (Corona) von 2019 bis 2022. 
+- Handelsvolumen (Price_sum blau) hat sich während Corona (ab 24.01.20) mehr als verdoppelt. 61,488 € zu 157,363 €
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Begründung:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Keine Präsenzauktionen mehr ab 07.03.2021
+- Median Anzahl_lots erhöht sich von 418 vor Corona auf 677,5 nach Corona
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Begründung:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Weine aus Präsenzauktionen werden in Onlineauktionen angeboten</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- Verkaufswahrscheinlichkeit erhöht sich von 73 % vor Corona auf 88 % nach Corona
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Begründung:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Nicht eindeutig. Gibt es mehr Käufer? Sind die Weine aus Präsenzauktionen, die jetzt online zusätzlich angeboten werden, begehrter?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Kritische Reflektion:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Datenpunkte vor Corona enthalten nur 8 Onlineauktionen</t>
+    </r>
+  </si>
+  <si>
+    <t>winepoints (descripition)</t>
+  </si>
+  <si>
+    <t>packaging</t>
+  </si>
+  <si>
+    <t>vintage</t>
+  </si>
+  <si>
+    <t>Analyse von Signalparameter (nicht qualitativ, nur ob diese angegeben sind oder nicht</t>
+  </si>
 </sst>
 </file>
 
@@ -75,7 +210,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +220,24 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -110,10 +263,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -536,297 +703,6 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Verkaufsvolumen nach Auktion'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>number_lots</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Verkaufsvolumen nach Auktion'!$A$2:$A$40</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>43513</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43563</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43653</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43737</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43749</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43828</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43877</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43952</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43955</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43968</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44054</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>44082</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>44101</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44172</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>44192</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44204</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44220</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>44241</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44265</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>44283</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44304</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44328</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44346</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>44367</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>44430</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>44444</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>44493</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>44507</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>44514</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>44539</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>44556</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>44566</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>44577</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>44619</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>44640</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>44703</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>44714</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>44838</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>44901</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Verkaufsvolumen nach Auktion'!$C$2:$C$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>380</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>722</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>584</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>305</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>518</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>418</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>319</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>494</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>248</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>323</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>478</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>779</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>508</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>473</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>735</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>628</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1047</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>638</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>691</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>776</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>569</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1246</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>950</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>567</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>522</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>892</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>822</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>671</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>1001</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>568</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>919</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>477</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>544</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>723</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>739</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>587</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>795</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>684</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>738</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-AB5B-45D9-A06C-2A17935F8D4B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
@@ -1408,297 +1284,6 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Verkaufsvolumen nach Auktion'!$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>prob_of_sale</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Verkaufsvolumen nach Auktion'!$A$2:$A$40</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>43513</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43563</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43653</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43737</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43749</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43828</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43877</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43952</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43955</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43968</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44054</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>44082</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>44101</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44172</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>44192</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44204</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44220</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>44241</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44265</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>44283</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44304</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44328</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44346</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>44367</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>44430</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>44444</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>44493</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>44507</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>44514</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>44539</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>44556</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>44566</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>44577</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>44619</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>44640</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>44703</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>44714</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>44838</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>44901</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Verkaufsvolumen nach Auktion'!$F$2:$F$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>0.72894736842105268</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.50277008310249305</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.58047945205479456</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.79016393442622945</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.66023166023166024</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.80622009569377995</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.84639498432601878</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.74291497975708498</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.80241935483870963</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.91950464396284826</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.79079497907949792</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.62772785622593064</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.70669291338582674</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.86257928118393234</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.77823129251700685</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.88216560509554143</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.92072588347659978</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.89341692789968652</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.93777134587554267</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.91237113402061853</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.94903339191564151</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.9357945425361156</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.88736842105263158</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.84303350970017632</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.86781609195402298</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>0.89125560538116588</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>0.90389294403892939</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>0.85991058122205666</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>0.82717282717282714</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.91725352112676062</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>0.82372143634385198</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0.89098532494758909</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.81066176470588236</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.8907330567081605</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.93234100135317999</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.77853492333901197</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.95597484276729561</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.86403508771929827</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.89701897018970189</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-EDDA-4EE7-93F0-B88142281847}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1711,6 +1296,632 @@
         <c:smooth val="0"/>
         <c:axId val="1210921184"/>
         <c:axId val="1210920352"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Verkaufsvolumen nach Auktion'!$C$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>number_lots</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="34925" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="000000">
+                        <a:alpha val="63000"/>
+                      </a:srgbClr>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Verkaufsvolumen nach Auktion'!$A$2:$A$40</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>m/d/yyyy</c:formatCode>
+                      <c:ptCount val="39"/>
+                      <c:pt idx="0">
+                        <c:v>43513</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>43563</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>43653</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>43737</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>43749</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>43828</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>43877</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>43952</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>43955</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>43968</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>44054</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>44082</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>44101</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>44172</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>44192</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>44204</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>44220</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>44241</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>44265</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>44283</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>44304</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>44328</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>44346</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>44367</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>44430</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>44444</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>44493</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>44507</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>44514</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>44539</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>44556</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>44566</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>44577</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>44619</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>44640</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>44703</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>44714</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>44838</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>44901</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Verkaufsvolumen nach Auktion'!$C$2:$C$40</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="39"/>
+                      <c:pt idx="0">
+                        <c:v>380</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>722</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>584</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>305</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>518</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>418</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>319</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>494</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>248</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>323</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>478</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>779</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>508</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>473</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>735</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>628</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>1047</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>638</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>691</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>776</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>569</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>1246</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>950</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>567</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>522</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>892</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>822</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>671</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>1001</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>568</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>919</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>477</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>544</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>723</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>739</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>587</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>795</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>684</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>738</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-AB5B-45D9-A06C-2A17935F8D4B}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Verkaufsvolumen nach Auktion'!$F$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>prob_of_sale</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="34925" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="000000">
+                        <a:alpha val="63000"/>
+                      </a:srgbClr>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Verkaufsvolumen nach Auktion'!$A$2:$A$40</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>m/d/yyyy</c:formatCode>
+                      <c:ptCount val="39"/>
+                      <c:pt idx="0">
+                        <c:v>43513</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>43563</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>43653</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>43737</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>43749</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>43828</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>43877</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>43952</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>43955</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>43968</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>44054</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>44082</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>44101</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>44172</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>44192</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>44204</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>44220</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>44241</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>44265</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>44283</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>44304</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>44328</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>44346</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>44367</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>44430</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>44444</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>44493</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>44507</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>44514</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>44539</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>44556</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>44566</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>44577</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>44619</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>44640</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>44703</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>44714</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>44838</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>44901</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Verkaufsvolumen nach Auktion'!$F$2:$F$40</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="39"/>
+                      <c:pt idx="0">
+                        <c:v>0.72894736842105268</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.50277008310249305</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>0.58047945205479456</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>0.79016393442622945</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>0.66023166023166024</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>0.80622009569377995</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0.84639498432601878</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>0.74291497975708498</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>0.80241935483870963</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>0.91950464396284826</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.79079497907949792</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.62772785622593064</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.70669291338582674</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>0.86257928118393234</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>0.77823129251700685</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>0.88216560509554143</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>0.92072588347659978</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>0.89341692789968652</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>0.93777134587554267</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>0.91237113402061853</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>0.94903339191564151</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>0.9357945425361156</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>0.88736842105263158</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>0.84303350970017632</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>0.86781609195402298</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>0.89125560538116588</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>0.90389294403892939</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>0.85991058122205666</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>0.82717282717282714</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>0.91725352112676062</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>0.82372143634385198</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>0.89098532494758909</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>0.81066176470588236</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>0.8907330567081605</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>0.93234100135317999</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>0.77853492333901197</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>0.95597484276729561</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>0.86403508771929827</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>0.89701897018970189</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-EDDA-4EE7-93F0-B88142281847}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:dateAx>
         <c:axId val="1210910784"/>
@@ -1966,6 +2177,7 @@
     <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -2056,297 +2268,6 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Verkaufsvolumen nach Auktion'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>price_sum</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="34925" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Verkaufsvolumen nach Auktion'!$A$2:$A$40</c:f>
-              <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>43513</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43563</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43653</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43737</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43749</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43828</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43877</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43952</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43955</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43968</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44054</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>44082</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>44101</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44172</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>44192</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>44204</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>44220</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>44241</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>44265</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>44283</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>44304</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>44328</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>44346</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>44367</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>44430</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>44444</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>44493</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>44507</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>44514</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>44539</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>44556</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>44566</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>44577</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>44619</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>44640</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>44703</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>44714</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>44838</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>44901</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Verkaufsvolumen nach Auktion'!$B$2:$B$40</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="39"/>
-                <c:pt idx="0">
-                  <c:v>47480.639999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>70193.524999999994</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>62836.890000000007</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43159.519999999997</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>61934.55</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>61488.78</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>45723</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>69844.149999999994</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>33916.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>55284.324999999997</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>59867.600000000006</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>96453.57</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>65128.425000000003</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>85400.5</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>132396.39000000001</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>186576.07500000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>312682.625</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>162494.50999999998</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>180885.71000000005</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>184112.19999999995</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>142627.02000000002</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>339684.17500000005</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>238349.48500000004</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>125924.94</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>116255.38499999999</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>216554.75000000003</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>233866.32500000004</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>162423.63</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>258483.755</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>156560.11499999999</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>195032.00500000003</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>132465.51</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>136946.73499999999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>158166.48999999993</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>171717.185</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>121046.02499999999</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>233480.88000000009</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>132586.18000000002</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>164519.505</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-73E1-4B71-B21F-9E893F45B3CD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2363,21 +2284,21 @@
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
+                <c:idx val="0"/>
+                <c:order val="0"/>
                 <c:tx>
                   <c:strRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Verkaufsvolumen nach Auktion'!$C$1</c15:sqref>
+                          <c15:sqref>'Verkaufsvolumen nach Auktion'!$B$1</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>number_lots</c:v>
+                        <c:v>price_sum</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -2385,7 +2306,7 @@
                 <c:spPr>
                   <a:ln w="34925" cap="rnd">
                     <a:solidFill>
-                      <a:schemeClr val="accent2"/>
+                      <a:schemeClr val="accent1"/>
                     </a:solidFill>
                     <a:round/>
                   </a:ln>
@@ -2537,6 +2458,317 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
+                          <c15:sqref>'Verkaufsvolumen nach Auktion'!$B$2:$B$40</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>#,##0.00\ "€"</c:formatCode>
+                      <c:ptCount val="39"/>
+                      <c:pt idx="0">
+                        <c:v>47480.639999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>70193.524999999994</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>62836.890000000007</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>43159.519999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>61934.55</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>61488.78</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>45723</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>69844.149999999994</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>33916.5</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>55284.324999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>59867.600000000006</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>96453.57</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>65128.425000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>85400.5</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>132396.39000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>186576.07500000001</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>312682.625</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>162494.50999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>180885.71000000005</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>184112.19999999995</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>142627.02000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>339684.17500000005</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>238349.48500000004</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>125924.94</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>116255.38499999999</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>216554.75000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>233866.32500000004</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>162423.63</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>258483.755</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>156560.11499999999</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>195032.00500000003</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>132465.51</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>136946.73499999999</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>158166.48999999993</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>171717.185</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>121046.02499999999</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>233480.88000000009</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>132586.18000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>164519.505</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-73E1-4B71-B21F-9E893F45B3CD}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Verkaufsvolumen nach Auktion'!$C$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>number_lots</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="34925" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst>
+                    <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                      <a:srgbClr val="000000">
+                        <a:alpha val="63000"/>
+                      </a:srgbClr>
+                    </a:outerShdw>
+                  </a:effectLst>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Verkaufsvolumen nach Auktion'!$A$2:$A$40</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>m/d/yyyy</c:formatCode>
+                      <c:ptCount val="39"/>
+                      <c:pt idx="0">
+                        <c:v>43513</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>43563</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>43653</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>43737</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>43749</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>43828</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>43877</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>43952</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>43955</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>43968</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>44054</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>44082</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>44101</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>44172</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>44192</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>44204</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>44220</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>44241</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>44265</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>44283</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>44304</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>44328</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>44346</c:v>
+                      </c:pt>
+                      <c:pt idx="23">
+                        <c:v>44367</c:v>
+                      </c:pt>
+                      <c:pt idx="24">
+                        <c:v>44430</c:v>
+                      </c:pt>
+                      <c:pt idx="25">
+                        <c:v>44444</c:v>
+                      </c:pt>
+                      <c:pt idx="26">
+                        <c:v>44493</c:v>
+                      </c:pt>
+                      <c:pt idx="27">
+                        <c:v>44507</c:v>
+                      </c:pt>
+                      <c:pt idx="28">
+                        <c:v>44514</c:v>
+                      </c:pt>
+                      <c:pt idx="29">
+                        <c:v>44539</c:v>
+                      </c:pt>
+                      <c:pt idx="30">
+                        <c:v>44556</c:v>
+                      </c:pt>
+                      <c:pt idx="31">
+                        <c:v>44566</c:v>
+                      </c:pt>
+                      <c:pt idx="32">
+                        <c:v>44577</c:v>
+                      </c:pt>
+                      <c:pt idx="33">
+                        <c:v>44619</c:v>
+                      </c:pt>
+                      <c:pt idx="34">
+                        <c:v>44640</c:v>
+                      </c:pt>
+                      <c:pt idx="35">
+                        <c:v>44703</c:v>
+                      </c:pt>
+                      <c:pt idx="36">
+                        <c:v>44714</c:v>
+                      </c:pt>
+                      <c:pt idx="37">
+                        <c:v>44838</c:v>
+                      </c:pt>
+                      <c:pt idx="38">
+                        <c:v>44901</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
                           <c15:sqref>'Verkaufsvolumen nach Auktion'!$C$2:$C$40</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
@@ -2665,7 +2897,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-73E1-4B71-B21F-9E893F45B3CD}"/>
                   </c:ext>
@@ -2976,7 +3208,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-73E1-4B71-B21F-9E893F45B3CD}"/>
                   </c:ext>
@@ -3287,7 +3519,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-73E1-4B71-B21F-9E893F45B3CD}"/>
                   </c:ext>
@@ -3604,7 +3836,7 @@
         <c:axId val="1210921184"/>
         <c:axId val="1210920352"/>
       </c:lineChart>
-      <c:dateAx>
+      <c:catAx>
         <c:axId val="1210910784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -3650,9 +3882,10 @@
         <c:crossAx val="1210920768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:baseTimeUnit val="days"/>
-      </c:dateAx>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="1210920768"/>
         <c:scaling>
@@ -3858,6 +4091,7 @@
     <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -5046,6 +5280,492 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.32</cdr:x>
+      <cdr:y>0.09905</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.32148</cdr:x>
+      <cdr:y>0.78398</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="3" name="Gerader Verbinder 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ABEAD09F-6ED8-809D-37DA-85415F30332E}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1" flipV="1">
+          <a:off x="2057400" y="447675"/>
+          <a:ext cx="9525" cy="3095625"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.31556</cdr:x>
+      <cdr:y>0.10959</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.47852</cdr:x>
+      <cdr:y>0.16649</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="Textfeld 3">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5DEC4E6-2F9E-5D8C-111A-68D17A0E5E02}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2028825" y="495300"/>
+          <a:ext cx="1047750" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Start</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> of Corona</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.57383</cdr:x>
+      <cdr:y>0.09975</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.57531</cdr:x>
+      <cdr:y>0.78469</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="5" name="Gerader Verbinder 4">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF85C447-EB87-4D48-A0FE-BB495D136A41}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1" flipV="1">
+          <a:off x="3689350" y="450850"/>
+          <a:ext cx="9525" cy="3095625"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.57235</cdr:x>
+      <cdr:y>0.11029</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.88</cdr:x>
+      <cdr:y>0.16719</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="Textfeld 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8EB6320-52D7-487A-F7D9-C1E59AC1F0B2}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3679824" y="498475"/>
+          <a:ext cx="1978025" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>No</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> In-person auctions anymore</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.28494</cdr:x>
+      <cdr:y>0.13616</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.28642</cdr:x>
+      <cdr:y>0.79339</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="2" name="Gerader Verbinder 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C053F999-5976-7FB4-B37D-BDFA1665C923}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1" flipV="1">
+          <a:off x="1831975" y="641350"/>
+          <a:ext cx="9525" cy="3095625"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+          <a:round/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.28049</cdr:x>
+      <cdr:y>0.14628</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.44346</cdr:x>
+      <cdr:y>0.20088</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="Textfeld 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FE9DC09-BC3B-EE53-DBD7-C2143619B667}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1803400" y="688975"/>
+          <a:ext cx="1047750" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Start</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> of Corona</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExterneDaten_1" connectionId="1" xr16:uid="{AF686096-9ECB-4121-B05C-2AF85773F93F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="7" unboundColumnsRight="3">
@@ -5341,23 +6061,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F6E698A-E8DB-4DEC-8095-0B474F0A20D2}">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q53" sqref="Q53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5376,8 +6097,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="Q1" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43513</v>
       </c>
@@ -5397,8 +6121,11 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.72894736842105268</v>
       </c>
+      <c r="Q2" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43563</v>
       </c>
@@ -5418,8 +6145,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.50277008310249305</v>
       </c>
+      <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43653</v>
       </c>
@@ -5439,8 +6167,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.58047945205479456</v>
       </c>
+      <c r="Q4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43737</v>
       </c>
@@ -5460,8 +6189,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.79016393442622945</v>
       </c>
+      <c r="Q5" s="4"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43749</v>
       </c>
@@ -5481,8 +6211,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.66023166023166024</v>
       </c>
+      <c r="Q6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43828</v>
       </c>
@@ -5502,8 +6233,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.80622009569377995</v>
       </c>
+      <c r="Q7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43877</v>
       </c>
@@ -5523,8 +6255,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.84639498432601878</v>
       </c>
+      <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>43952</v>
       </c>
@@ -5544,8 +6277,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.74291497975708498</v>
       </c>
+      <c r="Q9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43955</v>
       </c>
@@ -5565,8 +6299,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.80241935483870963</v>
       </c>
+      <c r="Q10" s="4"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43968</v>
       </c>
@@ -5586,8 +6321,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.91950464396284826</v>
       </c>
+      <c r="Q11" s="4"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44054</v>
       </c>
@@ -5607,8 +6343,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.79079497907949792</v>
       </c>
+      <c r="Q12" s="4"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44082</v>
       </c>
@@ -5628,8 +6365,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.62772785622593064</v>
       </c>
+      <c r="Q13" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44101</v>
       </c>
@@ -5649,8 +6387,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.70669291338582674</v>
       </c>
+      <c r="Q14" s="4"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44172</v>
       </c>
@@ -5670,8 +6409,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.86257928118393234</v>
       </c>
+      <c r="Q15" s="4"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44192</v>
       </c>
@@ -5691,8 +6431,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.77823129251700685</v>
       </c>
+      <c r="Q16" s="4"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44204</v>
       </c>
@@ -5712,8 +6453,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.88216560509554143</v>
       </c>
+      <c r="Q17" s="4"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44220</v>
       </c>
@@ -5733,8 +6475,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.92072588347659978</v>
       </c>
+      <c r="Q18" s="4"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44241</v>
       </c>
@@ -5754,8 +6497,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.89341692789968652</v>
       </c>
+      <c r="Q19" s="4"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44265</v>
       </c>
@@ -5775,8 +6519,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.93777134587554267</v>
       </c>
+      <c r="Q20" s="4"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44283</v>
       </c>
@@ -5796,8 +6541,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.91237113402061853</v>
       </c>
+      <c r="Q21" s="4"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44304</v>
       </c>
@@ -5817,8 +6563,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.94903339191564151</v>
       </c>
+      <c r="Q22" s="4"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44328</v>
       </c>
@@ -5838,8 +6585,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.9357945425361156</v>
       </c>
+      <c r="Q23" s="4"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44346</v>
       </c>
@@ -5859,8 +6607,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.88736842105263158</v>
       </c>
+      <c r="Q24" s="4"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44367</v>
       </c>
@@ -5881,7 +6630,7 @@
         <v>0.84303350970017632</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44430</v>
       </c>
@@ -5901,8 +6650,11 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.86781609195402298</v>
       </c>
+      <c r="Q26" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44444</v>
       </c>
@@ -5922,8 +6674,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.89125560538116588</v>
       </c>
+      <c r="Q27" s="5"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44493</v>
       </c>
@@ -5943,8 +6696,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.90389294403892939</v>
       </c>
+      <c r="Q28" s="5"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44507</v>
       </c>
@@ -5964,8 +6718,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.85991058122205666</v>
       </c>
+      <c r="Q29" s="5"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44514</v>
       </c>
@@ -5985,8 +6740,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.82717282717282714</v>
       </c>
+      <c r="Q30" s="5"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>44539</v>
       </c>
@@ -6006,8 +6762,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.91725352112676062</v>
       </c>
+      <c r="Q31" s="5"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>44556</v>
       </c>
@@ -6027,8 +6784,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.82372143634385198</v>
       </c>
+      <c r="Q32" s="5"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>44566</v>
       </c>
@@ -6048,8 +6806,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.89098532494758909</v>
       </c>
+      <c r="Q33" s="5"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>44577</v>
       </c>
@@ -6069,8 +6828,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.81066176470588236</v>
       </c>
+      <c r="Q34" s="5"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>44619</v>
       </c>
@@ -6090,8 +6850,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.8907330567081605</v>
       </c>
+      <c r="Q35" s="5"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>44640</v>
       </c>
@@ -6111,8 +6872,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.93234100135317999</v>
       </c>
+      <c r="Q36" s="5"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>44703</v>
       </c>
@@ -6132,8 +6894,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.77853492333901197</v>
       </c>
+      <c r="Q37" s="5"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>44714</v>
       </c>
@@ -6153,8 +6916,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.95597484276729561</v>
       </c>
+      <c r="Q38" s="5"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>44838</v>
       </c>
@@ -6174,8 +6938,9 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.86403508771929827</v>
       </c>
+      <c r="Q39" s="5"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>44901</v>
       </c>
@@ -6195,8 +6960,98 @@
         <f>data_1666209171584[[#This Row],[lot_sold]]/data_1666209171584[[#This Row],[number_lots]]</f>
         <v>0.89701897018970189</v>
       </c>
+      <c r="Q40" s="5"/>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q41" s="5"/>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q42" s="5"/>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q43" s="5"/>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="1">
+        <f>MEDIAN(B2:B8)</f>
+        <v>61488.78</v>
+      </c>
+      <c r="C44" s="7">
+        <f t="shared" ref="C44:F44" si="0">MEDIAN(C2:C8)</f>
+        <v>418</v>
+      </c>
+      <c r="D44" s="7">
+        <f t="shared" si="0"/>
+        <v>337</v>
+      </c>
+      <c r="E44" s="7">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+      <c r="F44" s="7">
+        <f t="shared" si="0"/>
+        <v>0.72894736842105268</v>
+      </c>
+      <c r="Q44" s="5"/>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="1">
+        <f>MEDIAN(B9:B40)</f>
+        <v>157363.30249999996</v>
+      </c>
+      <c r="C45" s="7">
+        <f t="shared" ref="C45:F45" si="1">MEDIAN(C9:C40)</f>
+        <v>677.5</v>
+      </c>
+      <c r="D45" s="7">
+        <f t="shared" si="1"/>
+        <v>571</v>
+      </c>
+      <c r="E45" s="7">
+        <f t="shared" si="1"/>
+        <v>79.5</v>
+      </c>
+      <c r="F45" s="7">
+        <f t="shared" si="1"/>
+        <v>0.88476701307408656</v>
+      </c>
+      <c r="Q45" s="5"/>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B46" s="2">
+        <v>44262</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q46" s="5"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q47" s="5"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q48" s="5"/>
+    </row>
+    <row r="49" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q49" s="5"/>
+    </row>
+    <row r="50" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q50" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="Q2:Q24"/>
+    <mergeCell ref="Q26:Q50"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -6209,12 +7064,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="2" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>